<commit_message>
Delete values from example/Brake System.xlsx
</commit_message>
<xml_diff>
--- a/example/Brake System.xlsx
+++ b/example/Brake System.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\KARTBOX_2020\Cost\Cost 2020\BOM\Brake System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryomei/Projects/cost-calculator/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4B540F-CA9D-44D9-A359-C0E03D156F66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B45B87E-0CAB-7345-A59F-7CA010FB2050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Summary" sheetId="18" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1294,7 +1297,7 @@
     <numFmt numFmtId="180" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2550,7 +2553,7 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1507.7463951185885</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>230.36999999999998</c:v>
@@ -3193,18 +3196,18 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="63" customWidth="1"/>
-    <col min="2" max="2" width="11.75" style="63" customWidth="1"/>
-    <col min="3" max="3" width="27.25" style="63" customWidth="1"/>
-    <col min="4" max="7" width="9.75" style="63" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" style="63" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="63" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="63" customWidth="1"/>
+    <col min="4" max="7" width="9.6640625" style="63" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="63" customWidth="1"/>
     <col min="9" max="9" width="3.5" style="63" customWidth="1"/>
-    <col min="10" max="16384" width="9.125" style="63"/>
+    <col min="10" max="16384" width="9.1640625" style="63"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="20">
       <c r="B2" s="176" t="s">
         <v>46</v>
       </c>
@@ -3215,7 +3218,7 @@
       <c r="G2" s="176"/>
       <c r="H2" s="176"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11">
       <c r="B4" s="64" t="s">
         <v>47</v>
       </c>
@@ -3225,14 +3228,14 @@
       </c>
       <c r="D4" s="177"/>
     </row>
-    <row r="5" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="33" customHeight="1">
       <c r="C5" s="178" t="str">
         <f>CONCATENATE("Car # ",BOM!B4)</f>
         <v>Car # 999</v>
       </c>
       <c r="D5" s="178"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11">
       <c r="B6" s="126" t="s">
         <v>146</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="15">
       <c r="B7" s="115">
         <v>1</v>
       </c>
@@ -3264,26 +3267,26 @@
       </c>
       <c r="D7" s="66">
         <f>BOM!J36</f>
-        <v>1312.9612661459068</v>
+        <v>0</v>
       </c>
       <c r="E7" s="66">
         <f>BOM!K36</f>
-        <v>191.712024238288</v>
+        <v>0</v>
       </c>
       <c r="F7" s="66">
         <f>BOM!L36</f>
-        <v>2.406438067726647</v>
+        <v>0</v>
       </c>
       <c r="G7" s="66">
         <f>BOM!M36</f>
-        <v>0.66666666666666696</v>
+        <v>0</v>
       </c>
       <c r="H7" s="66">
         <f>BOM!N36</f>
-        <v>1507.7463951185885</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15">
       <c r="B8" s="129">
         <v>2</v>
       </c>
@@ -3311,7 +3314,7 @@
         <v>230.36999999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="15">
       <c r="B9" s="132">
         <v>3</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>171.99</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="15">
       <c r="B10" s="135">
         <v>4</v>
       </c>
@@ -3367,7 +3370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="15">
       <c r="B11" s="138">
         <v>5</v>
       </c>
@@ -3395,7 +3398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15">
       <c r="B12" s="141">
         <v>6</v>
       </c>
@@ -3423,7 +3426,7 @@
         <v>47.97</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="15">
       <c r="B13" s="144">
         <v>7</v>
       </c>
@@ -3451,7 +3454,7 @@
         <v>124.4486671512</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="15">
       <c r="B14" s="147">
         <v>8</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11">
       <c r="B15" s="150"/>
       <c r="C15" s="150"/>
       <c r="D15" s="150"/>
@@ -3488,34 +3491,34 @@
       <c r="G15" s="150"/>
       <c r="H15" s="150"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11">
       <c r="B16" s="116"/>
       <c r="C16" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="117">
         <f>SUM(D7:D14)</f>
-        <v>1917.9685332971071</v>
+        <v>605.00726715120004</v>
       </c>
       <c r="E16" s="117">
         <f>SUM(E7:E14)</f>
-        <v>523.37342423828807</v>
+        <v>331.66140000000001</v>
       </c>
       <c r="F16" s="117">
         <f>SUM(F7:F14)</f>
-        <v>2.406438067726647</v>
+        <v>0</v>
       </c>
       <c r="G16" s="117">
         <f>SUM(G7:G14)</f>
-        <v>30.776666666666667</v>
+        <v>30.11</v>
       </c>
       <c r="H16" s="117">
         <f>SUM(H7:H14)</f>
-        <v>2474.5250622697886</v>
+        <v>966.77866715120001</v>
       </c>
       <c r="K16" s="67"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2">
       <c r="B19" s="63" t="s">
         <v>49</v>
       </c>
@@ -3556,27 +3559,27 @@
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7:M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="5" customWidth="1"/>
     <col min="4" max="4" width="10" style="79" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="29.875" style="61" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.75" style="5" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.75" style="8" customWidth="1"/>
-    <col min="10" max="13" width="10.625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.125" style="1"/>
+    <col min="9" max="9" width="5.6640625" style="8" customWidth="1"/>
+    <col min="10" max="13" width="10.6640625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="151" t="s">
         <v>5</v>
       </c>
@@ -3591,10 +3594,10 @@
       <c r="N1" s="153"/>
       <c r="O1" s="154">
         <f>N183</f>
-        <v>2474.5250622697886</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="83" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>966.77866715120001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="83" customFormat="1" ht="16" thickTop="1" thickBot="1">
       <c r="A2" s="152" t="s">
         <v>35</v>
       </c>
@@ -3604,7 +3607,7 @@
       <c r="C2" s="180"/>
       <c r="D2" s="82"/>
     </row>
-    <row r="3" spans="1:15" s="83" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="83" customFormat="1" ht="16" thickTop="1" thickBot="1">
       <c r="A3" s="151" t="s">
         <v>1</v>
       </c>
@@ -3614,7 +3617,7 @@
       <c r="C3" s="182"/>
       <c r="D3" s="82"/>
     </row>
-    <row r="4" spans="1:15" s="83" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="83" customFormat="1" ht="16" thickTop="1" thickBot="1">
       <c r="A4" s="151" t="s">
         <v>7</v>
       </c>
@@ -3626,13 +3629,13 @@
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="87" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="87" customFormat="1" ht="15" thickTop="1">
       <c r="A5" s="84"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
       <c r="D5" s="86"/>
     </row>
-    <row r="6" spans="1:15" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="51" customFormat="1" ht="30">
       <c r="A6" s="119" t="s">
         <v>43</v>
       </c>
@@ -3679,7 +3682,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="14">
       <c r="A7" s="166">
         <v>1</v>
       </c>
@@ -3698,31 +3701,21 @@
       </c>
       <c r="G7" s="169"/>
       <c r="H7" s="172">
-        <f>SUM(J7:M7)</f>
-        <v>3.625877067726647</v>
-      </c>
-      <c r="I7" s="173">
-        <v>1</v>
-      </c>
-      <c r="J7" s="172">
-        <v>0</v>
-      </c>
-      <c r="K7" s="172">
-        <v>3.25</v>
-      </c>
-      <c r="L7" s="172">
-        <v>0.37587706772664697</v>
-      </c>
-      <c r="M7" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" ref="H7:H35" si="0">SUM(J7:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="173"/>
+      <c r="J7" s="172"/>
+      <c r="K7" s="172"/>
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
       <c r="N7" s="174">
-        <f>H7*I7</f>
-        <v>3.625877067726647</v>
+        <f t="shared" ref="N7:N35" si="1">H7*I7</f>
+        <v>0</v>
       </c>
       <c r="O7" s="164"/>
     </row>
-    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="14">
       <c r="A8" s="166">
         <v>2</v>
       </c>
@@ -3743,31 +3736,21 @@
       </c>
       <c r="G8" s="169"/>
       <c r="H8" s="172">
-        <f>SUM(J8:M8)</f>
-        <v>50.815037500000003</v>
-      </c>
-      <c r="I8" s="173">
-        <v>1</v>
-      </c>
-      <c r="J8" s="172">
-        <v>48.940037500000003</v>
-      </c>
-      <c r="K8" s="172">
-        <v>1.875</v>
-      </c>
-      <c r="L8" s="172">
-        <v>0</v>
-      </c>
-      <c r="M8" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="173"/>
+      <c r="J8" s="172"/>
+      <c r="K8" s="172"/>
+      <c r="L8" s="172"/>
+      <c r="M8" s="172"/>
       <c r="N8" s="174">
-        <f>H8*I8</f>
-        <v>50.815037500000003</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O8" s="164"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14">
       <c r="A9" s="166">
         <v>3</v>
       </c>
@@ -3788,31 +3771,21 @@
       </c>
       <c r="G9" s="169"/>
       <c r="H9" s="172">
-        <f>SUM(J9:M9)</f>
-        <v>50.815037500000003</v>
-      </c>
-      <c r="I9" s="173">
-        <v>1</v>
-      </c>
-      <c r="J9" s="172">
-        <v>48.940037500000003</v>
-      </c>
-      <c r="K9" s="172">
-        <v>1.875</v>
-      </c>
-      <c r="L9" s="172">
-        <v>0</v>
-      </c>
-      <c r="M9" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="173"/>
+      <c r="J9" s="172"/>
+      <c r="K9" s="172"/>
+      <c r="L9" s="172"/>
+      <c r="M9" s="172"/>
       <c r="N9" s="174">
-        <f>H9*I9</f>
-        <v>50.815037500000003</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O9" s="164"/>
     </row>
-    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14">
       <c r="A10" s="166">
         <v>4</v>
       </c>
@@ -3833,31 +3806,21 @@
       </c>
       <c r="G10" s="169"/>
       <c r="H10" s="172">
-        <f>SUM(J10:M10)</f>
-        <v>6.7339454599999993</v>
-      </c>
-      <c r="I10" s="173">
-        <v>1</v>
-      </c>
-      <c r="J10" s="172">
-        <v>5.5939454599999996</v>
-      </c>
-      <c r="K10" s="172">
-        <v>1</v>
-      </c>
-      <c r="L10" s="172">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M10" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="173"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
+      <c r="M10" s="172"/>
       <c r="N10" s="174">
-        <f>H10*I10</f>
-        <v>6.7339454599999993</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O10" s="164"/>
     </row>
-    <row r="11" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A11" s="166">
         <v>5</v>
       </c>
@@ -3878,31 +3841,21 @@
       </c>
       <c r="G11" s="169"/>
       <c r="H11" s="172">
-        <f>SUM(J11:M11)</f>
-        <v>6.7339454599999993</v>
-      </c>
-      <c r="I11" s="173">
-        <v>1</v>
-      </c>
-      <c r="J11" s="172">
-        <v>5.5939454599999996</v>
-      </c>
-      <c r="K11" s="172">
-        <v>1</v>
-      </c>
-      <c r="L11" s="172">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M11" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="173"/>
+      <c r="J11" s="172"/>
+      <c r="K11" s="172"/>
+      <c r="L11" s="172"/>
+      <c r="M11" s="172"/>
       <c r="N11" s="174">
-        <f>H11*I11</f>
-        <v>6.7339454599999993</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O11" s="164"/>
     </row>
-    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14">
       <c r="A12" s="166">
         <v>6</v>
       </c>
@@ -3923,31 +3876,21 @@
       </c>
       <c r="G12" s="175"/>
       <c r="H12" s="172">
-        <f>SUM(J12:M12)</f>
-        <v>1.9833777883162145</v>
-      </c>
-      <c r="I12" s="173">
-        <v>2</v>
-      </c>
-      <c r="J12" s="172">
-        <v>9.6901797081446403E-3</v>
-      </c>
-      <c r="K12" s="172">
-        <v>1.9736876086080699</v>
-      </c>
-      <c r="L12" s="172">
-        <v>0</v>
-      </c>
-      <c r="M12" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="173"/>
+      <c r="J12" s="172"/>
+      <c r="K12" s="172"/>
+      <c r="L12" s="172"/>
+      <c r="M12" s="172"/>
       <c r="N12" s="174">
-        <f>H12*I12</f>
-        <v>3.9667555766324289</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O12" s="164"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14">
       <c r="A13" s="166">
         <v>7</v>
       </c>
@@ -3968,31 +3911,21 @@
       </c>
       <c r="G13" s="175"/>
       <c r="H13" s="172">
-        <f>SUM(J13:M13)</f>
-        <v>2.8239502677646202</v>
-      </c>
-      <c r="I13" s="173">
-        <v>1</v>
-      </c>
-      <c r="J13" s="172">
-        <v>6.7401600000000006E-2</v>
-      </c>
-      <c r="K13" s="172">
-        <v>2.75654866776462</v>
-      </c>
-      <c r="L13" s="172">
-        <v>0</v>
-      </c>
-      <c r="M13" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="173"/>
+      <c r="J13" s="172"/>
+      <c r="K13" s="172"/>
+      <c r="L13" s="172"/>
+      <c r="M13" s="172"/>
       <c r="N13" s="174">
-        <f>H13*I13</f>
-        <v>2.8239502677646202</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O13" s="164"/>
     </row>
-    <row r="14" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14">
       <c r="A14" s="166">
         <v>8</v>
       </c>
@@ -4013,31 +3946,21 @@
       </c>
       <c r="G14" s="175"/>
       <c r="H14" s="172">
-        <f>SUM(J14:M14)</f>
-        <v>7.7127508091663346</v>
-      </c>
-      <c r="I14" s="173">
-        <v>1</v>
-      </c>
-      <c r="J14" s="172">
-        <v>9.0415902344267995E-2</v>
-      </c>
-      <c r="K14" s="172">
-        <v>6.9556682401553998</v>
-      </c>
-      <c r="L14" s="172">
-        <v>0</v>
-      </c>
-      <c r="M14" s="172">
-        <v>0.66666666666666696</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="173"/>
+      <c r="J14" s="172"/>
+      <c r="K14" s="172"/>
+      <c r="L14" s="172"/>
+      <c r="M14" s="172"/>
       <c r="N14" s="174">
-        <f>H14*I14</f>
-        <v>7.7127508091663346</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O14" s="164"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14">
       <c r="A15" s="166">
         <v>9</v>
       </c>
@@ -4058,31 +3981,21 @@
       </c>
       <c r="G15" s="175"/>
       <c r="H15" s="172">
-        <f>SUM(J15:M15)</f>
-        <v>1.6273124000000001</v>
-      </c>
-      <c r="I15" s="173">
-        <v>1</v>
-      </c>
-      <c r="J15" s="172">
-        <v>1.5422399999999999E-2</v>
-      </c>
-      <c r="K15" s="172">
-        <v>1.61189</v>
-      </c>
-      <c r="L15" s="172">
-        <v>0</v>
-      </c>
-      <c r="M15" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="173"/>
+      <c r="J15" s="172"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="172"/>
+      <c r="M15" s="172"/>
       <c r="N15" s="174">
-        <f>H15*I15</f>
-        <v>1.6273124000000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O15" s="164"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14">
       <c r="A16" s="166">
         <v>10</v>
       </c>
@@ -4101,31 +4014,21 @@
       </c>
       <c r="G16" s="175"/>
       <c r="H16" s="172">
-        <f>SUM(J16:M16)</f>
-        <v>1.625</v>
-      </c>
-      <c r="I16" s="173">
-        <v>1</v>
-      </c>
-      <c r="J16" s="172">
-        <v>0</v>
-      </c>
-      <c r="K16" s="172">
-        <v>1.625</v>
-      </c>
-      <c r="L16" s="172">
-        <v>0</v>
-      </c>
-      <c r="M16" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="173"/>
+      <c r="J16" s="172"/>
+      <c r="K16" s="172"/>
+      <c r="L16" s="172"/>
+      <c r="M16" s="172"/>
       <c r="N16" s="174">
-        <f>H16*I16</f>
-        <v>1.625</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O16" s="164"/>
     </row>
-    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="14">
       <c r="A17" s="166">
         <v>11</v>
       </c>
@@ -4146,31 +4049,21 @@
       </c>
       <c r="G17" s="175"/>
       <c r="H17" s="172">
-        <f>SUM(J17:M17)</f>
-        <v>30</v>
-      </c>
-      <c r="I17" s="173">
-        <v>1</v>
-      </c>
-      <c r="J17" s="172">
-        <v>30</v>
-      </c>
-      <c r="K17" s="172">
-        <v>0</v>
-      </c>
-      <c r="L17" s="172">
-        <v>0</v>
-      </c>
-      <c r="M17" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="173"/>
+      <c r="J17" s="172"/>
+      <c r="K17" s="172"/>
+      <c r="L17" s="172"/>
+      <c r="M17" s="172"/>
       <c r="N17" s="174">
-        <f>H17*I17</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O17" s="164"/>
     </row>
-    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="14">
       <c r="A18" s="166">
         <v>12</v>
       </c>
@@ -4191,31 +4084,21 @@
       </c>
       <c r="G18" s="175"/>
       <c r="H18" s="172">
-        <f>SUM(J18:M18)</f>
-        <v>26</v>
-      </c>
-      <c r="I18" s="173">
-        <v>1</v>
-      </c>
-      <c r="J18" s="172">
-        <v>26</v>
-      </c>
-      <c r="K18" s="172">
-        <v>0</v>
-      </c>
-      <c r="L18" s="172">
-        <v>0</v>
-      </c>
-      <c r="M18" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="173"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
+      <c r="L18" s="172"/>
+      <c r="M18" s="172"/>
       <c r="N18" s="174">
-        <f>H18*I18</f>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O18" s="164"/>
     </row>
-    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="14">
       <c r="A19" s="166">
         <v>13</v>
       </c>
@@ -4234,31 +4117,21 @@
       </c>
       <c r="G19" s="175"/>
       <c r="H19" s="172">
-        <f>SUM(J19:M19)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="173">
-        <v>1</v>
-      </c>
-      <c r="J19" s="172">
-        <v>0</v>
-      </c>
-      <c r="K19" s="172">
-        <v>0</v>
-      </c>
-      <c r="L19" s="172">
-        <v>0</v>
-      </c>
-      <c r="M19" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="173"/>
+      <c r="J19" s="172"/>
+      <c r="K19" s="172"/>
+      <c r="L19" s="172"/>
+      <c r="M19" s="172"/>
       <c r="N19" s="174">
-        <f>H19*I19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O19" s="164"/>
     </row>
-    <row r="20" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="14">
       <c r="A20" s="166">
         <v>14</v>
       </c>
@@ -4279,31 +4152,21 @@
       </c>
       <c r="G20" s="175"/>
       <c r="H20" s="172">
-        <f>SUM(J20:M20)</f>
-        <v>56.886571437500002</v>
-      </c>
-      <c r="I20" s="173">
-        <v>1</v>
-      </c>
-      <c r="J20" s="172">
-        <v>53.011571437500002</v>
-      </c>
-      <c r="K20" s="172">
-        <v>3.875</v>
-      </c>
-      <c r="L20" s="172">
-        <v>0</v>
-      </c>
-      <c r="M20" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="173"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="172"/>
+      <c r="L20" s="172"/>
+      <c r="M20" s="172"/>
       <c r="N20" s="174">
-        <f>H20*I20</f>
-        <v>56.886571437500002</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O20" s="164"/>
     </row>
-    <row r="21" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="14">
       <c r="A21" s="166">
         <v>15</v>
       </c>
@@ -4322,31 +4185,21 @@
       </c>
       <c r="G21" s="158"/>
       <c r="H21" s="161">
-        <f>SUM(J21:M21)</f>
-        <v>0.87528050000000002</v>
-      </c>
-      <c r="I21" s="162">
-        <v>2</v>
-      </c>
-      <c r="J21" s="161">
-        <v>0</v>
-      </c>
-      <c r="K21" s="161">
-        <v>0</v>
-      </c>
-      <c r="L21" s="161">
-        <v>0.87528050000000002</v>
-      </c>
-      <c r="M21" s="161">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="162"/>
+      <c r="J21" s="161"/>
+      <c r="K21" s="161"/>
+      <c r="L21" s="161"/>
+      <c r="M21" s="161"/>
       <c r="N21" s="163">
-        <f>H21*I21</f>
-        <v>1.750561</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O21" s="164"/>
     </row>
-    <row r="22" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="14">
       <c r="A22" s="166">
         <v>16</v>
       </c>
@@ -4367,31 +4220,21 @@
       </c>
       <c r="G22" s="158"/>
       <c r="H22" s="161">
-        <f>SUM(J22:M22)</f>
-        <v>12.635000083234889</v>
-      </c>
-      <c r="I22" s="162">
-        <v>2</v>
-      </c>
-      <c r="J22" s="161">
-        <v>1.3401581870871899</v>
-      </c>
-      <c r="K22" s="161">
-        <v>11.2948418961477</v>
-      </c>
-      <c r="L22" s="161">
-        <v>0</v>
-      </c>
-      <c r="M22" s="161">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="162"/>
+      <c r="J22" s="161"/>
+      <c r="K22" s="161"/>
+      <c r="L22" s="161"/>
+      <c r="M22" s="161"/>
       <c r="N22" s="163">
-        <f>H22*I22</f>
-        <v>25.270000166469778</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O22" s="164"/>
     </row>
-    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="14">
       <c r="A23" s="166">
         <v>17</v>
       </c>
@@ -4412,31 +4255,21 @@
       </c>
       <c r="G23" s="169"/>
       <c r="H23" s="172">
-        <f>SUM(J23:M23)</f>
-        <v>15.774129253398591</v>
-      </c>
-      <c r="I23" s="173">
-        <v>2</v>
-      </c>
-      <c r="J23" s="172">
-        <v>2.48744639851629</v>
-      </c>
-      <c r="K23" s="172">
-        <v>13.286682854882301</v>
-      </c>
-      <c r="L23" s="172">
-        <v>0</v>
-      </c>
-      <c r="M23" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="173"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="172"/>
+      <c r="L23" s="172"/>
+      <c r="M23" s="172"/>
       <c r="N23" s="174">
-        <f>H23*I23</f>
-        <v>31.548258506797183</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O23" s="164"/>
     </row>
-    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="14">
       <c r="A24" s="166">
         <v>18</v>
       </c>
@@ -4457,31 +4290,21 @@
       </c>
       <c r="G24" s="169"/>
       <c r="H24" s="172">
-        <f>SUM(J24:M24)</f>
-        <v>2.1455257004501718</v>
-      </c>
-      <c r="I24" s="173">
-        <v>24</v>
-      </c>
-      <c r="J24" s="172">
-        <v>5.3414423924561798E-2</v>
-      </c>
-      <c r="K24" s="172">
-        <v>2.09211127652561</v>
-      </c>
-      <c r="L24" s="172">
-        <v>0</v>
-      </c>
-      <c r="M24" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="173"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="172"/>
+      <c r="L24" s="172"/>
+      <c r="M24" s="172"/>
       <c r="N24" s="174">
-        <f>H24*I24</f>
-        <v>51.492616810804122</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O24" s="164"/>
     </row>
-    <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="14">
       <c r="A25" s="166">
         <v>19</v>
       </c>
@@ -4500,31 +4323,21 @@
       </c>
       <c r="G25" s="175"/>
       <c r="H25" s="172">
-        <f>SUM(J25:M25)</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="173">
-        <v>2</v>
-      </c>
-      <c r="J25" s="172">
-        <v>0</v>
-      </c>
-      <c r="K25" s="172">
-        <v>0</v>
-      </c>
-      <c r="L25" s="172">
-        <v>0</v>
-      </c>
-      <c r="M25" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="173"/>
+      <c r="J25" s="172"/>
+      <c r="K25" s="172"/>
+      <c r="L25" s="172"/>
+      <c r="M25" s="172"/>
       <c r="N25" s="174">
-        <f>H25*I25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O25" s="164"/>
     </row>
-    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="14">
       <c r="A26" s="166">
         <v>20</v>
       </c>
@@ -4545,31 +4358,21 @@
       </c>
       <c r="G26" s="175"/>
       <c r="H26" s="172">
-        <f>SUM(J26:M26)</f>
-        <v>156.55216098723861</v>
-      </c>
-      <c r="I26" s="173">
-        <v>2</v>
-      </c>
-      <c r="J26" s="172">
-        <v>151.08125000000001</v>
-      </c>
-      <c r="K26" s="172">
-        <v>5.4709109872385904</v>
-      </c>
-      <c r="L26" s="172">
-        <v>0</v>
-      </c>
-      <c r="M26" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="173"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="172"/>
+      <c r="L26" s="172"/>
+      <c r="M26" s="172"/>
       <c r="N26" s="174">
-        <f>H26*I26</f>
-        <v>313.10432197447722</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O26" s="164"/>
     </row>
-    <row r="27" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="14">
       <c r="A27" s="166">
         <v>21</v>
       </c>
@@ -4590,31 +4393,21 @@
       </c>
       <c r="G27" s="175"/>
       <c r="H27" s="172">
-        <f>SUM(J27:M27)</f>
-        <v>50.315037500000003</v>
-      </c>
-      <c r="I27" s="173">
-        <v>2</v>
-      </c>
-      <c r="J27" s="172">
-        <v>48.440037500000003</v>
-      </c>
-      <c r="K27" s="172">
-        <v>1.875</v>
-      </c>
-      <c r="L27" s="172">
-        <v>0</v>
-      </c>
-      <c r="M27" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="173"/>
+      <c r="J27" s="172"/>
+      <c r="K27" s="172"/>
+      <c r="L27" s="172"/>
+      <c r="M27" s="172"/>
       <c r="N27" s="174">
-        <f>H27*I27</f>
-        <v>100.63007500000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O27" s="164"/>
     </row>
-    <row r="28" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="14">
       <c r="A28" s="166">
         <v>22</v>
       </c>
@@ -4633,31 +4426,21 @@
       </c>
       <c r="G28" s="175"/>
       <c r="H28" s="172">
-        <f>SUM(J28:M28)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="173">
-        <v>2</v>
-      </c>
-      <c r="J28" s="172">
-        <v>0</v>
-      </c>
-      <c r="K28" s="172">
-        <v>0</v>
-      </c>
-      <c r="L28" s="172">
-        <v>0</v>
-      </c>
-      <c r="M28" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="173"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="172"/>
+      <c r="M28" s="172"/>
       <c r="N28" s="174">
-        <f>H28*I28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O28" s="164"/>
     </row>
-    <row r="29" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="14">
       <c r="A29" s="166">
         <v>23</v>
       </c>
@@ -4678,31 +4461,21 @@
       </c>
       <c r="G29" s="175"/>
       <c r="H29" s="172">
-        <f>SUM(J29:M29)</f>
-        <v>0.24432000000000001</v>
-      </c>
-      <c r="I29" s="173">
-        <v>4</v>
-      </c>
-      <c r="J29" s="172">
-        <v>0.24432000000000001</v>
-      </c>
-      <c r="K29" s="172">
-        <v>0</v>
-      </c>
-      <c r="L29" s="172">
-        <v>0</v>
-      </c>
-      <c r="M29" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="173"/>
+      <c r="J29" s="172"/>
+      <c r="K29" s="172"/>
+      <c r="L29" s="172"/>
+      <c r="M29" s="172"/>
       <c r="N29" s="174">
-        <f>H29*I29</f>
-        <v>0.97728000000000004</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O29" s="164"/>
     </row>
-    <row r="30" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="14">
       <c r="A30" s="166">
         <v>24</v>
       </c>
@@ -4723,31 +4496,21 @@
       </c>
       <c r="G30" s="175"/>
       <c r="H30" s="172">
-        <f>SUM(J30:M30)</f>
-        <v>0.26456000000000002</v>
-      </c>
-      <c r="I30" s="173">
-        <v>4</v>
-      </c>
-      <c r="J30" s="172">
-        <v>0.26456000000000002</v>
-      </c>
-      <c r="K30" s="172">
-        <v>0</v>
-      </c>
-      <c r="L30" s="172">
-        <v>0</v>
-      </c>
-      <c r="M30" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="173"/>
+      <c r="J30" s="172"/>
+      <c r="K30" s="172"/>
+      <c r="L30" s="172"/>
+      <c r="M30" s="172"/>
       <c r="N30" s="174">
-        <f>H30*I30</f>
-        <v>1.0582400000000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O30" s="164"/>
     </row>
-    <row r="31" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="14">
       <c r="A31" s="166">
         <v>25</v>
       </c>
@@ -4766,31 +4529,21 @@
       </c>
       <c r="G31" s="169"/>
       <c r="H31" s="172">
-        <f>SUM(J31:M31)</f>
-        <v>0.27</v>
-      </c>
-      <c r="I31" s="173">
-        <v>1</v>
-      </c>
-      <c r="J31" s="172">
-        <v>0.27</v>
-      </c>
-      <c r="K31" s="172">
-        <v>0</v>
-      </c>
-      <c r="L31" s="172">
-        <v>0</v>
-      </c>
-      <c r="M31" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="173"/>
+      <c r="J31" s="172"/>
+      <c r="K31" s="172"/>
+      <c r="L31" s="172"/>
+      <c r="M31" s="172"/>
       <c r="N31" s="174">
-        <f>H31*I31</f>
-        <v>0.27</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O31" s="164"/>
     </row>
-    <row r="32" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="14">
       <c r="A32" s="166">
         <v>26</v>
       </c>
@@ -4809,31 +4562,21 @@
       </c>
       <c r="G32" s="169"/>
       <c r="H32" s="172">
-        <f>SUM(J32:M32)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="173">
-        <v>1</v>
-      </c>
-      <c r="J32" s="172">
-        <v>0</v>
-      </c>
-      <c r="K32" s="172">
-        <v>0</v>
-      </c>
-      <c r="L32" s="172">
-        <v>0</v>
-      </c>
-      <c r="M32" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="173"/>
+      <c r="J32" s="172"/>
+      <c r="K32" s="172"/>
+      <c r="L32" s="172"/>
+      <c r="M32" s="172"/>
       <c r="N32" s="174">
-        <f>H32*I32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O32" s="164"/>
     </row>
-    <row r="33" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="14">
       <c r="A33" s="166">
         <v>27</v>
       </c>
@@ -4854,31 +4597,21 @@
       </c>
       <c r="G33" s="169"/>
       <c r="H33" s="172">
-        <f>SUM(J33:M33)</f>
-        <v>272.157831875</v>
-      </c>
-      <c r="I33" s="173">
-        <v>1</v>
-      </c>
-      <c r="J33" s="172">
-        <v>253.032831875</v>
-      </c>
-      <c r="K33" s="172">
-        <v>19.125</v>
-      </c>
-      <c r="L33" s="172">
-        <v>0</v>
-      </c>
-      <c r="M33" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="173"/>
+      <c r="J33" s="172"/>
+      <c r="K33" s="172"/>
+      <c r="L33" s="172"/>
+      <c r="M33" s="172"/>
       <c r="N33" s="174">
-        <f>H33*I33</f>
-        <v>272.157831875</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O33" s="164"/>
     </row>
-    <row r="34" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="14">
       <c r="A34" s="166">
         <v>28</v>
       </c>
@@ -4899,31 +4632,21 @@
       </c>
       <c r="G34" s="169"/>
       <c r="H34" s="172">
-        <f>SUM(J34:M34)</f>
-        <v>31.754956875000001</v>
-      </c>
-      <c r="I34" s="173">
-        <v>1</v>
-      </c>
-      <c r="J34" s="172">
-        <v>27.879956875000001</v>
-      </c>
-      <c r="K34" s="172">
-        <v>3.875</v>
-      </c>
-      <c r="L34" s="172">
-        <v>0</v>
-      </c>
-      <c r="M34" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="173"/>
+      <c r="J34" s="172"/>
+      <c r="K34" s="172"/>
+      <c r="L34" s="172"/>
+      <c r="M34" s="172"/>
       <c r="N34" s="174">
-        <f>H34*I34</f>
-        <v>31.754956875000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O34" s="164"/>
     </row>
-    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15" thickBot="1">
       <c r="A35" s="166">
         <v>29</v>
       </c>
@@ -4944,31 +4667,21 @@
       </c>
       <c r="G35" s="169"/>
       <c r="H35" s="172">
-        <f>SUM(J35:M35)</f>
-        <v>428.36606943125003</v>
-      </c>
-      <c r="I35" s="173">
-        <v>1</v>
-      </c>
-      <c r="J35" s="172">
-        <v>403.49106943125003</v>
-      </c>
-      <c r="K35" s="172">
-        <v>24.875</v>
-      </c>
-      <c r="L35" s="172">
-        <v>0</v>
-      </c>
-      <c r="M35" s="172">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="173"/>
+      <c r="J35" s="172"/>
+      <c r="K35" s="172"/>
+      <c r="L35" s="172"/>
+      <c r="M35" s="172"/>
       <c r="N35" s="174">
-        <f>H35*I35</f>
-        <v>428.36606943125003</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O35" s="164"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A36" s="9"/>
       <c r="B36" s="53" t="s">
         <v>11</v>
@@ -4984,27 +4697,27 @@
       <c r="I36" s="90"/>
       <c r="J36" s="98">
         <f>SUMPRODUCT(I7:I35,J7:J35)</f>
-        <v>1312.9612661459068</v>
+        <v>0</v>
       </c>
       <c r="K36" s="98">
         <f>SUMPRODUCT(I7:I35,K7:K35)</f>
-        <v>191.712024238288</v>
+        <v>0</v>
       </c>
       <c r="L36" s="98">
         <f>SUMPRODUCT(I7:I35,L7:L35)</f>
-        <v>2.406438067726647</v>
+        <v>0</v>
       </c>
       <c r="M36" s="98">
         <f>SUMPRODUCT(I7:I35,M7:M35)</f>
-        <v>0.66666666666666696</v>
+        <v>0</v>
       </c>
       <c r="N36" s="99">
         <f>SUM(N7:N35)</f>
-        <v>1507.7463951185885</v>
+        <v>0</v>
       </c>
       <c r="O36" s="12"/>
     </row>
-    <row r="37" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15" thickTop="1">
       <c r="A37" s="13">
         <v>10</v>
       </c>
@@ -5032,12 +4745,12 @@
       <c r="L37" s="101"/>
       <c r="M37" s="101"/>
       <c r="N37" s="107">
-        <f t="shared" ref="N37:N80" si="0">H37*I37</f>
+        <f t="shared" ref="N37:N80" si="2">H37*I37</f>
         <v>0</v>
       </c>
       <c r="O37" s="16"/>
     </row>
-    <row r="38" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="14">
       <c r="A38" s="13">
         <v>20</v>
       </c>
@@ -5056,7 +4769,7 @@
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="15">
-        <f t="shared" ref="H38:H112" si="1">SUM(J38:M38)</f>
+        <f t="shared" ref="H38:H112" si="3">SUM(J38:M38)</f>
         <v>0</v>
       </c>
       <c r="I38" s="91"/>
@@ -5065,12 +4778,12 @@
       <c r="L38" s="101"/>
       <c r="M38" s="101"/>
       <c r="N38" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O38" s="16"/>
     </row>
-    <row r="39" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="14">
       <c r="A39" s="13">
         <v>30</v>
       </c>
@@ -5089,7 +4802,7 @@
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I39" s="91"/>
@@ -5098,12 +4811,12 @@
       <c r="L39" s="101"/>
       <c r="M39" s="101"/>
       <c r="N39" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O39" s="16"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="14">
       <c r="A40" s="13">
         <v>40</v>
       </c>
@@ -5122,7 +4835,7 @@
       </c>
       <c r="G40" s="14"/>
       <c r="H40" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I40" s="91"/>
@@ -5131,12 +4844,12 @@
       <c r="L40" s="101"/>
       <c r="M40" s="101"/>
       <c r="N40" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O40" s="16"/>
     </row>
-    <row r="41" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="14">
       <c r="A41" s="13">
         <v>50</v>
       </c>
@@ -5155,7 +4868,7 @@
       </c>
       <c r="G41" s="14"/>
       <c r="H41" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I41" s="91"/>
@@ -5164,12 +4877,12 @@
       <c r="L41" s="101"/>
       <c r="M41" s="101"/>
       <c r="N41" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O41" s="16"/>
     </row>
-    <row r="42" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="14">
       <c r="A42" s="13">
         <v>60</v>
       </c>
@@ -5188,7 +4901,7 @@
       </c>
       <c r="G42" s="14"/>
       <c r="H42" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I42" s="91"/>
@@ -5197,12 +4910,12 @@
       <c r="L42" s="101"/>
       <c r="M42" s="101"/>
       <c r="N42" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O42" s="16"/>
     </row>
-    <row r="43" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="14">
       <c r="A43" s="13">
         <v>70</v>
       </c>
@@ -5221,7 +4934,7 @@
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I43" s="91"/>
@@ -5230,12 +4943,12 @@
       <c r="L43" s="101"/>
       <c r="M43" s="101"/>
       <c r="N43" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O43" s="16"/>
     </row>
-    <row r="44" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="14">
       <c r="A44" s="13">
         <v>80</v>
       </c>
@@ -5254,7 +4967,7 @@
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I44" s="91"/>
@@ -5263,12 +4976,12 @@
       <c r="L44" s="101"/>
       <c r="M44" s="101"/>
       <c r="N44" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O44" s="16"/>
     </row>
-    <row r="45" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="14">
       <c r="A45" s="13">
         <v>90</v>
       </c>
@@ -5287,7 +5000,7 @@
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I45" s="91"/>
@@ -5296,12 +5009,12 @@
       <c r="L45" s="101"/>
       <c r="M45" s="101"/>
       <c r="N45" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="14">
       <c r="A46" s="13">
         <v>100</v>
       </c>
@@ -5320,7 +5033,7 @@
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>230.36999999999998</v>
       </c>
       <c r="I46" s="91">
@@ -5337,12 +5050,12 @@
         <v>24.66</v>
       </c>
       <c r="N46" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>230.36999999999998</v>
       </c>
       <c r="O46" s="16"/>
     </row>
-    <row r="47" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="14">
       <c r="A47" s="13">
         <v>110</v>
       </c>
@@ -5361,7 +5074,7 @@
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I47" s="91"/>
@@ -5370,12 +5083,12 @@
       <c r="L47" s="101"/>
       <c r="M47" s="101"/>
       <c r="N47" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O47" s="16"/>
     </row>
-    <row r="48" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="14">
       <c r="A48" s="13">
         <v>120</v>
       </c>
@@ -5394,7 +5107,7 @@
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="15">
-        <f t="shared" ref="H48:H52" si="2">SUM(J48:M48)</f>
+        <f t="shared" ref="H48:H52" si="4">SUM(J48:M48)</f>
         <v>0</v>
       </c>
       <c r="I48" s="91"/>
@@ -5403,12 +5116,12 @@
       <c r="L48" s="101"/>
       <c r="M48" s="101"/>
       <c r="N48" s="107">
-        <f t="shared" ref="N48:N52" si="3">H48*I48</f>
+        <f t="shared" ref="N48:N52" si="5">H48*I48</f>
         <v>0</v>
       </c>
       <c r="O48" s="16"/>
     </row>
-    <row r="49" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="14">
       <c r="A49" s="13">
         <v>130</v>
       </c>
@@ -5427,7 +5140,7 @@
       </c>
       <c r="G49" s="14"/>
       <c r="H49" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I49" s="91"/>
@@ -5436,12 +5149,12 @@
       <c r="L49" s="101"/>
       <c r="M49" s="101"/>
       <c r="N49" s="107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O49" s="16"/>
     </row>
-    <row r="50" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="14">
       <c r="A50" s="13">
         <v>140</v>
       </c>
@@ -5460,7 +5173,7 @@
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I50" s="91"/>
@@ -5469,12 +5182,12 @@
       <c r="L50" s="101"/>
       <c r="M50" s="101"/>
       <c r="N50" s="107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O50" s="16"/>
     </row>
-    <row r="51" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A51" s="13">
         <v>150</v>
       </c>
@@ -5495,7 +5208,7 @@
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I51" s="91"/>
@@ -5504,12 +5217,12 @@
       <c r="L51" s="101"/>
       <c r="M51" s="101"/>
       <c r="N51" s="107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O51" s="16"/>
     </row>
-    <row r="52" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="14">
       <c r="A52" s="13">
         <v>160</v>
       </c>
@@ -5530,7 +5243,7 @@
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I52" s="91"/>
@@ -5539,12 +5252,12 @@
       <c r="L52" s="101"/>
       <c r="M52" s="101"/>
       <c r="N52" s="107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O52" s="16"/>
     </row>
-    <row r="53" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="14">
       <c r="A53" s="13">
         <v>170</v>
       </c>
@@ -5565,7 +5278,7 @@
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I53" s="91"/>
@@ -5574,12 +5287,12 @@
       <c r="L53" s="101"/>
       <c r="M53" s="101"/>
       <c r="N53" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O53" s="16"/>
     </row>
-    <row r="54" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="14">
       <c r="A54" s="13">
         <v>180</v>
       </c>
@@ -5598,7 +5311,7 @@
       </c>
       <c r="G54" s="14"/>
       <c r="H54" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I54" s="91"/>
@@ -5607,12 +5320,12 @@
       <c r="L54" s="101"/>
       <c r="M54" s="101"/>
       <c r="N54" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O54" s="16"/>
     </row>
-    <row r="55" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="14">
       <c r="A55" s="13">
         <v>190</v>
       </c>
@@ -5631,7 +5344,7 @@
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I55" s="91"/>
@@ -5640,12 +5353,12 @@
       <c r="L55" s="101"/>
       <c r="M55" s="101"/>
       <c r="N55" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O55" s="16"/>
     </row>
-    <row r="56" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="14">
       <c r="A56" s="13">
         <v>200</v>
       </c>
@@ -5664,7 +5377,7 @@
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I56" s="91"/>
@@ -5673,12 +5386,12 @@
       <c r="L56" s="101"/>
       <c r="M56" s="101"/>
       <c r="N56" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O56" s="16"/>
     </row>
-    <row r="57" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="14">
       <c r="A57" s="13">
         <v>210</v>
       </c>
@@ -5697,7 +5410,7 @@
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I57" s="91"/>
@@ -5706,12 +5419,12 @@
       <c r="L57" s="101"/>
       <c r="M57" s="101"/>
       <c r="N57" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O57" s="16"/>
     </row>
-    <row r="58" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="14">
       <c r="A58" s="13">
         <v>220</v>
       </c>
@@ -5730,7 +5443,7 @@
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I58" s="91"/>
@@ -5739,12 +5452,12 @@
       <c r="L58" s="101"/>
       <c r="M58" s="101"/>
       <c r="N58" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O58" s="16"/>
     </row>
-    <row r="59" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="14">
       <c r="A59" s="13">
         <v>230</v>
       </c>
@@ -5763,7 +5476,7 @@
       </c>
       <c r="G59" s="17"/>
       <c r="H59" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I59" s="91"/>
@@ -5772,12 +5485,12 @@
       <c r="L59" s="101"/>
       <c r="M59" s="101"/>
       <c r="N59" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O59" s="16"/>
     </row>
-    <row r="60" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="14">
       <c r="A60" s="13">
         <v>240</v>
       </c>
@@ -5796,7 +5509,7 @@
       </c>
       <c r="G60" s="14"/>
       <c r="H60" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I60" s="91"/>
@@ -5805,12 +5518,12 @@
       <c r="L60" s="101"/>
       <c r="M60" s="101"/>
       <c r="N60" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O60" s="16"/>
     </row>
-    <row r="61" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="14">
       <c r="A61" s="13">
         <v>250</v>
       </c>
@@ -5829,7 +5542,7 @@
       </c>
       <c r="G61" s="14"/>
       <c r="H61" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I61" s="91"/>
@@ -5838,12 +5551,12 @@
       <c r="L61" s="101"/>
       <c r="M61" s="101"/>
       <c r="N61" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O61" s="16"/>
     </row>
-    <row r="62" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="14">
       <c r="A62" s="13">
         <v>260</v>
       </c>
@@ -5876,7 +5589,7 @@
       </c>
       <c r="O62" s="16"/>
     </row>
-    <row r="63" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="14">
       <c r="A63" s="13">
         <v>270</v>
       </c>
@@ -5895,7 +5608,7 @@
       </c>
       <c r="G63" s="14"/>
       <c r="H63" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I63" s="91"/>
@@ -5904,12 +5617,12 @@
       <c r="L63" s="101"/>
       <c r="M63" s="101"/>
       <c r="N63" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O63" s="16"/>
     </row>
-    <row r="64" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="14">
       <c r="A64" s="13">
         <v>280</v>
       </c>
@@ -5928,7 +5641,7 @@
       </c>
       <c r="G64" s="14"/>
       <c r="H64" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I64" s="91"/>
@@ -5937,12 +5650,12 @@
       <c r="L64" s="101"/>
       <c r="M64" s="101"/>
       <c r="N64" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O64" s="16"/>
     </row>
-    <row r="65" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="14">
       <c r="A65" s="13">
         <v>290</v>
       </c>
@@ -5961,7 +5674,7 @@
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I65" s="91"/>
@@ -5970,12 +5683,12 @@
       <c r="L65" s="101"/>
       <c r="M65" s="101"/>
       <c r="N65" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O65" s="16"/>
     </row>
-    <row r="66" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="14">
       <c r="A66" s="13">
         <v>300</v>
       </c>
@@ -5994,7 +5707,7 @@
       </c>
       <c r="G66" s="14"/>
       <c r="H66" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I66" s="91"/>
@@ -6003,12 +5716,12 @@
       <c r="L66" s="101"/>
       <c r="M66" s="101"/>
       <c r="N66" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O66" s="16"/>
     </row>
-    <row r="67" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A67" s="13">
         <v>310</v>
       </c>
@@ -6027,7 +5740,7 @@
       </c>
       <c r="G67" s="14"/>
       <c r="H67" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I67" s="91"/>
@@ -6036,12 +5749,12 @@
       <c r="L67" s="101"/>
       <c r="M67" s="101"/>
       <c r="N67" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O67" s="16"/>
     </row>
-    <row r="68" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="14">
       <c r="A68" s="13">
         <v>320</v>
       </c>
@@ -6062,7 +5775,7 @@
       </c>
       <c r="G68" s="14"/>
       <c r="H68" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I68" s="91"/>
@@ -6071,12 +5784,12 @@
       <c r="L68" s="101"/>
       <c r="M68" s="101"/>
       <c r="N68" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O68" s="16"/>
     </row>
-    <row r="69" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="14">
       <c r="A69" s="13">
         <v>330</v>
       </c>
@@ -6097,7 +5810,7 @@
       </c>
       <c r="G69" s="14"/>
       <c r="H69" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I69" s="91"/>
@@ -6106,12 +5819,12 @@
       <c r="L69" s="101"/>
       <c r="M69" s="101"/>
       <c r="N69" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O69" s="16"/>
     </row>
-    <row r="70" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="14">
       <c r="A70" s="13">
         <v>340</v>
       </c>
@@ -6132,7 +5845,7 @@
       </c>
       <c r="G70" s="14"/>
       <c r="H70" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I70" s="91"/>
@@ -6141,12 +5854,12 @@
       <c r="L70" s="101"/>
       <c r="M70" s="101"/>
       <c r="N70" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O70" s="16"/>
     </row>
-    <row r="71" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="14">
       <c r="A71" s="13">
         <v>350</v>
       </c>
@@ -6176,12 +5889,12 @@
       <c r="L71" s="101"/>
       <c r="M71" s="101"/>
       <c r="N71" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O71" s="16"/>
     </row>
-    <row r="72" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="14">
       <c r="A72" s="13">
         <v>360</v>
       </c>
@@ -6202,7 +5915,7 @@
       </c>
       <c r="G72" s="14"/>
       <c r="H72" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I72" s="91"/>
@@ -6216,7 +5929,7 @@
       </c>
       <c r="O72" s="16"/>
     </row>
-    <row r="73" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="14">
       <c r="A73" s="13">
         <v>370</v>
       </c>
@@ -6249,7 +5962,7 @@
       </c>
       <c r="O73" s="16"/>
     </row>
-    <row r="74" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="14">
       <c r="A74" s="13">
         <v>380</v>
       </c>
@@ -6282,7 +5995,7 @@
       </c>
       <c r="O74" s="16"/>
     </row>
-    <row r="75" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" ht="14">
       <c r="A75" s="13">
         <v>390</v>
       </c>
@@ -6301,7 +6014,7 @@
       </c>
       <c r="G75" s="14"/>
       <c r="H75" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I75" s="91"/>
@@ -6310,12 +6023,12 @@
       <c r="L75" s="101"/>
       <c r="M75" s="101"/>
       <c r="N75" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O75" s="16"/>
     </row>
-    <row r="76" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="14">
       <c r="A76" s="13">
         <v>400</v>
       </c>
@@ -6336,7 +6049,7 @@
       </c>
       <c r="G76" s="14"/>
       <c r="H76" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I76" s="91"/>
@@ -6345,12 +6058,12 @@
       <c r="L76" s="101"/>
       <c r="M76" s="101"/>
       <c r="N76" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O76" s="16"/>
     </row>
-    <row r="77" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="14">
       <c r="A77" s="13">
         <v>410</v>
       </c>
@@ -6371,7 +6084,7 @@
       </c>
       <c r="G77" s="14"/>
       <c r="H77" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I77" s="91"/>
@@ -6380,12 +6093,12 @@
       <c r="L77" s="101"/>
       <c r="M77" s="101"/>
       <c r="N77" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O77" s="16"/>
     </row>
-    <row r="78" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="14">
       <c r="A78" s="13">
         <v>420</v>
       </c>
@@ -6406,7 +6119,7 @@
       </c>
       <c r="G78" s="14"/>
       <c r="H78" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I78" s="91"/>
@@ -6415,12 +6128,12 @@
       <c r="L78" s="101"/>
       <c r="M78" s="101"/>
       <c r="N78" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O78" s="16"/>
     </row>
-    <row r="79" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" ht="14">
       <c r="A79" s="13">
         <v>430</v>
       </c>
@@ -6441,7 +6154,7 @@
       </c>
       <c r="G79" s="14"/>
       <c r="H79" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I79" s="91"/>
@@ -6450,12 +6163,12 @@
       <c r="L79" s="101"/>
       <c r="M79" s="101"/>
       <c r="N79" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O79" s="16"/>
     </row>
-    <row r="80" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="15" thickBot="1">
       <c r="A80" s="13">
         <v>440</v>
       </c>
@@ -6476,7 +6189,7 @@
       </c>
       <c r="G80" s="14"/>
       <c r="H80" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I80" s="91"/>
@@ -6485,12 +6198,12 @@
       <c r="L80" s="101"/>
       <c r="M80" s="101"/>
       <c r="N80" s="107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O80" s="16"/>
     </row>
-    <row r="81" spans="1:15" s="2" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="2" customFormat="1" ht="16" thickTop="1" thickBot="1">
       <c r="A81" s="9"/>
       <c r="B81" s="53" t="s">
         <v>15</v>
@@ -6526,7 +6239,7 @@
       </c>
       <c r="O81" s="12"/>
     </row>
-    <row r="82" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="15" thickTop="1">
       <c r="A82" s="19">
         <v>10</v>
       </c>
@@ -6554,12 +6267,12 @@
       <c r="L82" s="102"/>
       <c r="M82" s="102"/>
       <c r="N82" s="108">
-        <f t="shared" ref="N82:N96" si="4">H82*I82</f>
+        <f t="shared" ref="N82:N96" si="6">H82*I82</f>
         <v>0</v>
       </c>
       <c r="O82" s="22"/>
     </row>
-    <row r="83" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" ht="14">
       <c r="A83" s="19">
         <v>20</v>
       </c>
@@ -6587,12 +6300,12 @@
       <c r="L83" s="102"/>
       <c r="M83" s="102"/>
       <c r="N83" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O83" s="22"/>
     </row>
-    <row r="84" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="14">
       <c r="A84" s="19">
         <v>30</v>
       </c>
@@ -6628,12 +6341,12 @@
         <v>4.45</v>
       </c>
       <c r="N84" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>171.99</v>
       </c>
       <c r="O84" s="22"/>
     </row>
-    <row r="85" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="14">
       <c r="A85" s="19">
         <v>40</v>
       </c>
@@ -6661,12 +6374,12 @@
       <c r="L85" s="102"/>
       <c r="M85" s="102"/>
       <c r="N85" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O85" s="22"/>
     </row>
-    <row r="86" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" ht="14">
       <c r="A86" s="19">
         <v>50</v>
       </c>
@@ -6699,7 +6412,7 @@
       </c>
       <c r="O86" s="22"/>
     </row>
-    <row r="87" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" ht="14">
       <c r="A87" s="19">
         <v>60</v>
       </c>
@@ -6718,7 +6431,7 @@
       </c>
       <c r="G87" s="20"/>
       <c r="H87" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I87" s="92"/>
@@ -6727,12 +6440,12 @@
       <c r="L87" s="102"/>
       <c r="M87" s="102"/>
       <c r="N87" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O87" s="22"/>
     </row>
-    <row r="88" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="14">
       <c r="A88" s="19">
         <v>70</v>
       </c>
@@ -6760,12 +6473,12 @@
       <c r="L88" s="102"/>
       <c r="M88" s="102"/>
       <c r="N88" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O88" s="22"/>
     </row>
-    <row r="89" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="14">
       <c r="A89" s="19">
         <v>80</v>
       </c>
@@ -6784,7 +6497,7 @@
       </c>
       <c r="G89" s="20"/>
       <c r="H89" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I89" s="92"/>
@@ -6793,12 +6506,12 @@
       <c r="L89" s="102"/>
       <c r="M89" s="102"/>
       <c r="N89" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O89" s="22"/>
     </row>
-    <row r="90" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="14">
       <c r="A90" s="19">
         <v>90</v>
       </c>
@@ -6831,7 +6544,7 @@
       </c>
       <c r="O90" s="22"/>
     </row>
-    <row r="91" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A91" s="19">
         <v>100</v>
       </c>
@@ -6850,7 +6563,7 @@
       </c>
       <c r="G91" s="20"/>
       <c r="H91" s="21">
-        <f t="shared" ref="H91:H95" si="5">SUM(J91:M91)</f>
+        <f t="shared" ref="H91:H95" si="7">SUM(J91:M91)</f>
         <v>0</v>
       </c>
       <c r="I91" s="92"/>
@@ -6859,12 +6572,12 @@
       <c r="L91" s="102"/>
       <c r="M91" s="102"/>
       <c r="N91" s="108">
-        <f t="shared" ref="N91:N95" si="6">H91*I91</f>
+        <f t="shared" ref="N91:N95" si="8">H91*I91</f>
         <v>0</v>
       </c>
       <c r="O91" s="22"/>
     </row>
-    <row r="92" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="14">
       <c r="A92" s="19">
         <v>110</v>
       </c>
@@ -6883,7 +6596,7 @@
       </c>
       <c r="G92" s="20"/>
       <c r="H92" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I92" s="92"/>
@@ -6892,12 +6605,12 @@
       <c r="L92" s="102"/>
       <c r="M92" s="102"/>
       <c r="N92" s="108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O92" s="22"/>
     </row>
-    <row r="93" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="14">
       <c r="A93" s="19">
         <v>120</v>
       </c>
@@ -6916,7 +6629,7 @@
       </c>
       <c r="G93" s="20"/>
       <c r="H93" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I93" s="92"/>
@@ -6925,12 +6638,12 @@
       <c r="L93" s="102"/>
       <c r="M93" s="102"/>
       <c r="N93" s="108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O93" s="22"/>
     </row>
-    <row r="94" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" ht="14">
       <c r="A94" s="19">
         <v>130</v>
       </c>
@@ -6949,7 +6662,7 @@
       </c>
       <c r="G94" s="20"/>
       <c r="H94" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I94" s="92"/>
@@ -6958,12 +6671,12 @@
       <c r="L94" s="102"/>
       <c r="M94" s="102"/>
       <c r="N94" s="108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O94" s="22"/>
     </row>
-    <row r="95" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="14">
       <c r="A95" s="19">
         <v>140</v>
       </c>
@@ -6982,7 +6695,7 @@
       </c>
       <c r="G95" s="20"/>
       <c r="H95" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I95" s="92"/>
@@ -6991,12 +6704,12 @@
       <c r="L95" s="102"/>
       <c r="M95" s="102"/>
       <c r="N95" s="108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O95" s="22"/>
     </row>
-    <row r="96" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="15" thickBot="1">
       <c r="A96" s="19">
         <v>150</v>
       </c>
@@ -7024,12 +6737,12 @@
       <c r="L96" s="102"/>
       <c r="M96" s="102"/>
       <c r="N96" s="108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O96" s="22"/>
     </row>
-    <row r="97" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A97" s="9"/>
       <c r="B97" s="53" t="s">
         <v>22</v>
@@ -7065,7 +6778,7 @@
       </c>
       <c r="O97" s="12"/>
     </row>
-    <row r="98" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" ht="15" thickTop="1">
       <c r="A98" s="24">
         <v>10</v>
       </c>
@@ -7084,7 +6797,7 @@
       </c>
       <c r="G98" s="28"/>
       <c r="H98" s="26">
-        <f t="shared" ref="H98:H104" si="7">SUM(J98:M98)</f>
+        <f t="shared" ref="H98:H104" si="9">SUM(J98:M98)</f>
         <v>0</v>
       </c>
       <c r="I98" s="93"/>
@@ -7093,12 +6806,12 @@
       <c r="L98" s="103"/>
       <c r="M98" s="103"/>
       <c r="N98" s="109">
-        <f t="shared" ref="N98:N110" si="8">H98*I98</f>
+        <f t="shared" ref="N98:N110" si="10">H98*I98</f>
         <v>0</v>
       </c>
       <c r="O98" s="27"/>
     </row>
-    <row r="99" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" ht="14">
       <c r="A99" s="24">
         <v>20</v>
       </c>
@@ -7117,7 +6830,7 @@
       </c>
       <c r="G99" s="28"/>
       <c r="H99" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I99" s="93"/>
@@ -7126,12 +6839,12 @@
       <c r="L99" s="103"/>
       <c r="M99" s="103"/>
       <c r="N99" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O99" s="27"/>
     </row>
-    <row r="100" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" ht="14">
       <c r="A100" s="24">
         <v>30</v>
       </c>
@@ -7150,7 +6863,7 @@
       </c>
       <c r="G100" s="28"/>
       <c r="H100" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I100" s="93"/>
@@ -7159,12 +6872,12 @@
       <c r="L100" s="103"/>
       <c r="M100" s="103"/>
       <c r="N100" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O100" s="27"/>
     </row>
-    <row r="101" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" ht="14">
       <c r="A101" s="24">
         <v>40</v>
       </c>
@@ -7183,7 +6896,7 @@
       </c>
       <c r="G101" s="28"/>
       <c r="H101" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I101" s="93"/>
@@ -7192,12 +6905,12 @@
       <c r="L101" s="103"/>
       <c r="M101" s="103"/>
       <c r="N101" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O101" s="27"/>
     </row>
-    <row r="102" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" ht="14">
       <c r="A102" s="24">
         <v>50</v>
       </c>
@@ -7216,7 +6929,7 @@
       </c>
       <c r="G102" s="28"/>
       <c r="H102" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I102" s="93"/>
@@ -7225,12 +6938,12 @@
       <c r="L102" s="103"/>
       <c r="M102" s="103"/>
       <c r="N102" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O102" s="27"/>
     </row>
-    <row r="103" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" ht="14">
       <c r="A103" s="24">
         <v>60</v>
       </c>
@@ -7249,7 +6962,7 @@
       </c>
       <c r="G103" s="28"/>
       <c r="H103" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I103" s="93"/>
@@ -7258,12 +6971,12 @@
       <c r="L103" s="103"/>
       <c r="M103" s="103"/>
       <c r="N103" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O103" s="27"/>
     </row>
-    <row r="104" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" ht="14">
       <c r="A104" s="24">
         <v>70</v>
       </c>
@@ -7282,7 +6995,7 @@
       </c>
       <c r="G104" s="28"/>
       <c r="H104" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I104" s="93"/>
@@ -7291,12 +7004,12 @@
       <c r="L104" s="103"/>
       <c r="M104" s="103"/>
       <c r="N104" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O104" s="27"/>
     </row>
-    <row r="105" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A105" s="24">
         <v>80</v>
       </c>
@@ -7315,7 +7028,7 @@
       </c>
       <c r="G105" s="28"/>
       <c r="H105" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I105" s="93">
@@ -7328,12 +7041,12 @@
       <c r="L105" s="103"/>
       <c r="M105" s="103"/>
       <c r="N105" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="O105" s="27"/>
     </row>
-    <row r="106" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" ht="14">
       <c r="A106" s="24">
         <v>90</v>
       </c>
@@ -7352,7 +7065,7 @@
       </c>
       <c r="G106" s="28"/>
       <c r="H106" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I106" s="93"/>
@@ -7361,12 +7074,12 @@
       <c r="L106" s="103"/>
       <c r="M106" s="103"/>
       <c r="N106" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O106" s="27"/>
     </row>
-    <row r="107" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" ht="14">
       <c r="A107" s="24">
         <v>100</v>
       </c>
@@ -7385,7 +7098,7 @@
       </c>
       <c r="G107" s="25"/>
       <c r="H107" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="I107" s="93">
@@ -7398,12 +7111,12 @@
       <c r="L107" s="103"/>
       <c r="M107" s="103"/>
       <c r="N107" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="O107" s="27"/>
     </row>
-    <row r="108" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" ht="14">
       <c r="A108" s="24">
         <v>110</v>
       </c>
@@ -7422,7 +7135,7 @@
       </c>
       <c r="G108" s="28"/>
       <c r="H108" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I108" s="93"/>
@@ -7431,12 +7144,12 @@
       <c r="L108" s="103"/>
       <c r="M108" s="103"/>
       <c r="N108" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O108" s="27"/>
     </row>
-    <row r="109" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" ht="14">
       <c r="A109" s="24">
         <v>120</v>
       </c>
@@ -7469,7 +7182,7 @@
       </c>
       <c r="O109" s="27"/>
     </row>
-    <row r="110" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="15" thickBot="1">
       <c r="A110" s="24">
         <v>130</v>
       </c>
@@ -7488,7 +7201,7 @@
       </c>
       <c r="G110" s="25"/>
       <c r="H110" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I110" s="93"/>
@@ -7497,12 +7210,12 @@
       <c r="L110" s="103"/>
       <c r="M110" s="103"/>
       <c r="N110" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O110" s="27"/>
     </row>
-    <row r="111" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A111" s="9"/>
       <c r="B111" s="53" t="s">
         <v>42</v>
@@ -7538,7 +7251,7 @@
       </c>
       <c r="O111" s="12"/>
     </row>
-    <row r="112" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" ht="15" thickTop="1">
       <c r="A112" s="29">
         <v>10</v>
       </c>
@@ -7557,7 +7270,7 @@
       </c>
       <c r="G112" s="30"/>
       <c r="H112" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I112" s="94"/>
@@ -7566,12 +7279,12 @@
       <c r="L112" s="104"/>
       <c r="M112" s="104"/>
       <c r="N112" s="110">
-        <f t="shared" ref="N112:N120" si="9">H112*I112</f>
+        <f t="shared" ref="N112:N120" si="11">H112*I112</f>
         <v>0</v>
       </c>
       <c r="O112" s="32"/>
     </row>
-    <row r="113" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15" ht="14">
       <c r="A113" s="29">
         <v>20</v>
       </c>
@@ -7590,7 +7303,7 @@
       </c>
       <c r="G113" s="30"/>
       <c r="H113" s="31">
-        <f t="shared" ref="H113:H120" si="10">SUM(J113:M113)</f>
+        <f t="shared" ref="H113:H120" si="12">SUM(J113:M113)</f>
         <v>0</v>
       </c>
       <c r="I113" s="94"/>
@@ -7599,12 +7312,12 @@
       <c r="L113" s="104"/>
       <c r="M113" s="104"/>
       <c r="N113" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O113" s="32"/>
     </row>
-    <row r="114" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15" ht="14">
       <c r="A114" s="29">
         <v>30</v>
       </c>
@@ -7623,7 +7336,7 @@
       </c>
       <c r="G114" s="30"/>
       <c r="H114" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="I114" s="94">
@@ -7636,12 +7349,12 @@
       <c r="L114" s="104"/>
       <c r="M114" s="104"/>
       <c r="N114" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="O114" s="32"/>
     </row>
-    <row r="115" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:15" ht="14">
       <c r="A115" s="29">
         <v>40</v>
       </c>
@@ -7660,7 +7373,7 @@
       </c>
       <c r="G115" s="30"/>
       <c r="H115" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I115" s="94"/>
@@ -7669,12 +7382,12 @@
       <c r="L115" s="104"/>
       <c r="M115" s="104"/>
       <c r="N115" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O115" s="32"/>
     </row>
-    <row r="116" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" ht="14">
       <c r="A116" s="29">
         <v>50</v>
       </c>
@@ -7693,7 +7406,7 @@
       </c>
       <c r="G116" s="30"/>
       <c r="H116" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I116" s="94"/>
@@ -7702,12 +7415,12 @@
       <c r="L116" s="104"/>
       <c r="M116" s="104"/>
       <c r="N116" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O116" s="32"/>
     </row>
-    <row r="117" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" ht="14">
       <c r="A117" s="29">
         <v>60</v>
       </c>
@@ -7726,7 +7439,7 @@
       </c>
       <c r="G117" s="30"/>
       <c r="H117" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I117" s="94"/>
@@ -7735,12 +7448,12 @@
       <c r="L117" s="104"/>
       <c r="M117" s="104"/>
       <c r="N117" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O117" s="32"/>
     </row>
-    <row r="118" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" ht="14">
       <c r="A118" s="29">
         <v>70</v>
       </c>
@@ -7759,7 +7472,7 @@
       </c>
       <c r="G118" s="30"/>
       <c r="H118" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I118" s="94"/>
@@ -7768,12 +7481,12 @@
       <c r="L118" s="104"/>
       <c r="M118" s="104"/>
       <c r="N118" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O118" s="32"/>
     </row>
-    <row r="119" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" ht="14">
       <c r="A119" s="29">
         <v>80</v>
       </c>
@@ -7792,7 +7505,7 @@
       </c>
       <c r="G119" s="30"/>
       <c r="H119" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I119" s="94"/>
@@ -7801,12 +7514,12 @@
       <c r="L119" s="104"/>
       <c r="M119" s="104"/>
       <c r="N119" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O119" s="32"/>
     </row>
-    <row r="120" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="15" thickBot="1">
       <c r="A120" s="29">
         <v>90</v>
       </c>
@@ -7825,7 +7538,7 @@
       </c>
       <c r="G120" s="30"/>
       <c r="H120" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I120" s="94"/>
@@ -7834,12 +7547,12 @@
       <c r="L120" s="104"/>
       <c r="M120" s="104"/>
       <c r="N120" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O120" s="32"/>
     </row>
-    <row r="121" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A121" s="9"/>
       <c r="B121" s="53" t="s">
         <v>84</v>
@@ -7875,7 +7588,7 @@
       </c>
       <c r="O121" s="12"/>
     </row>
-    <row r="122" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" ht="15" thickTop="1">
       <c r="A122" s="33">
         <v>10</v>
       </c>
@@ -7908,7 +7621,7 @@
       </c>
       <c r="O122" s="36"/>
     </row>
-    <row r="123" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" ht="14">
       <c r="A123" s="33">
         <v>20</v>
       </c>
@@ -7929,7 +7642,7 @@
       </c>
       <c r="G123" s="34"/>
       <c r="H123" s="35">
-        <f t="shared" ref="H123:H133" si="11">SUM(J123:M123)</f>
+        <f t="shared" ref="H123:H133" si="13">SUM(J123:M123)</f>
         <v>0</v>
       </c>
       <c r="I123" s="95"/>
@@ -7938,12 +7651,12 @@
       <c r="L123" s="105"/>
       <c r="M123" s="105"/>
       <c r="N123" s="111">
-        <f t="shared" ref="N123:N133" si="12">H123*I123</f>
+        <f t="shared" ref="N123:N133" si="14">H123*I123</f>
         <v>0</v>
       </c>
       <c r="O123" s="36"/>
     </row>
-    <row r="124" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" ht="14">
       <c r="A124" s="33">
         <v>30</v>
       </c>
@@ -7964,7 +7677,7 @@
       </c>
       <c r="G124" s="34"/>
       <c r="H124" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I124" s="95"/>
@@ -7973,12 +7686,12 @@
       <c r="L124" s="105"/>
       <c r="M124" s="105"/>
       <c r="N124" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O124" s="36"/>
     </row>
-    <row r="125" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" ht="14">
       <c r="A125" s="33">
         <v>40</v>
       </c>
@@ -7999,7 +7712,7 @@
       </c>
       <c r="G125" s="34"/>
       <c r="H125" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I125" s="95"/>
@@ -8008,12 +7721,12 @@
       <c r="L125" s="105"/>
       <c r="M125" s="105"/>
       <c r="N125" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O125" s="36"/>
     </row>
-    <row r="126" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" ht="14">
       <c r="A126" s="33">
         <v>50</v>
       </c>
@@ -8032,7 +7745,7 @@
       </c>
       <c r="G126" s="34"/>
       <c r="H126" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I126" s="95"/>
@@ -8041,12 +7754,12 @@
       <c r="L126" s="105"/>
       <c r="M126" s="105"/>
       <c r="N126" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O126" s="36"/>
     </row>
-    <row r="127" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" ht="14">
       <c r="A127" s="33">
         <v>60</v>
       </c>
@@ -8067,7 +7780,7 @@
       </c>
       <c r="G127" s="34"/>
       <c r="H127" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I127" s="95"/>
@@ -8076,12 +7789,12 @@
       <c r="L127" s="105"/>
       <c r="M127" s="105"/>
       <c r="N127" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O127" s="36"/>
     </row>
-    <row r="128" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" ht="14">
       <c r="A128" s="33">
         <v>70</v>
       </c>
@@ -8102,7 +7815,7 @@
       </c>
       <c r="G128" s="34"/>
       <c r="H128" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I128" s="95"/>
@@ -8111,12 +7824,12 @@
       <c r="L128" s="105"/>
       <c r="M128" s="105"/>
       <c r="N128" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O128" s="36"/>
     </row>
-    <row r="129" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" ht="14">
       <c r="A129" s="33">
         <v>80</v>
       </c>
@@ -8135,7 +7848,7 @@
       </c>
       <c r="G129" s="34"/>
       <c r="H129" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I129" s="95"/>
@@ -8144,12 +7857,12 @@
       <c r="L129" s="105"/>
       <c r="M129" s="105"/>
       <c r="N129" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O129" s="36"/>
     </row>
-    <row r="130" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" ht="14">
       <c r="A130" s="33">
         <v>90</v>
       </c>
@@ -8170,7 +7883,7 @@
       </c>
       <c r="G130" s="34"/>
       <c r="H130" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I130" s="95"/>
@@ -8179,12 +7892,12 @@
       <c r="L130" s="105"/>
       <c r="M130" s="105"/>
       <c r="N130" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O130" s="36"/>
     </row>
-    <row r="131" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" ht="14">
       <c r="A131" s="33">
         <v>100</v>
       </c>
@@ -8205,7 +7918,7 @@
       </c>
       <c r="G131" s="34"/>
       <c r="H131" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I131" s="95"/>
@@ -8214,12 +7927,12 @@
       <c r="L131" s="105"/>
       <c r="M131" s="105"/>
       <c r="N131" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O131" s="36"/>
     </row>
-    <row r="132" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" ht="14">
       <c r="A132" s="33">
         <v>110</v>
       </c>
@@ -8254,7 +7967,7 @@
       </c>
       <c r="O132" s="36"/>
     </row>
-    <row r="133" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" ht="14">
       <c r="A133" s="33">
         <v>120</v>
       </c>
@@ -8273,7 +7986,7 @@
       </c>
       <c r="G133" s="34"/>
       <c r="H133" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>47.97</v>
       </c>
       <c r="I133" s="95">
@@ -8288,12 +8001,12 @@
       <c r="L133" s="105"/>
       <c r="M133" s="105"/>
       <c r="N133" s="111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>47.97</v>
       </c>
       <c r="O133" s="36"/>
     </row>
-    <row r="134" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="15" thickBot="1">
       <c r="A134" s="33">
         <v>130</v>
       </c>
@@ -8326,7 +8039,7 @@
       </c>
       <c r="O134" s="36"/>
     </row>
-    <row r="135" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A135" s="9"/>
       <c r="B135" s="53" t="s">
         <v>29</v>
@@ -8362,7 +8075,7 @@
       </c>
       <c r="O135" s="12"/>
     </row>
-    <row r="136" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" ht="15" thickTop="1">
       <c r="A136" s="38">
         <v>10</v>
       </c>
@@ -8381,7 +8094,7 @@
       </c>
       <c r="G136" s="39"/>
       <c r="H136" s="40">
-        <f t="shared" ref="H136:H163" si="13">SUM(J136:M136)</f>
+        <f t="shared" ref="H136:H163" si="15">SUM(J136:M136)</f>
         <v>0</v>
       </c>
       <c r="I136" s="96"/>
@@ -8390,12 +8103,12 @@
       <c r="L136" s="100"/>
       <c r="M136" s="100"/>
       <c r="N136" s="112">
-        <f t="shared" ref="N136:N163" si="14">H136*I136</f>
+        <f t="shared" ref="N136:N163" si="16">H136*I136</f>
         <v>0</v>
       </c>
       <c r="O136" s="41"/>
     </row>
-    <row r="137" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A137" s="38">
         <v>20</v>
       </c>
@@ -8414,7 +8127,7 @@
       </c>
       <c r="G137" s="39"/>
       <c r="H137" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I137" s="96"/>
@@ -8423,12 +8136,12 @@
       <c r="L137" s="100"/>
       <c r="M137" s="100"/>
       <c r="N137" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O137" s="41"/>
     </row>
-    <row r="138" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15" ht="14">
       <c r="A138" s="38">
         <v>30</v>
       </c>
@@ -8447,7 +8160,7 @@
       </c>
       <c r="G138" s="39"/>
       <c r="H138" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I138" s="96"/>
@@ -8456,12 +8169,12 @@
       <c r="L138" s="100"/>
       <c r="M138" s="100"/>
       <c r="N138" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O138" s="41"/>
     </row>
-    <row r="139" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:15" ht="14">
       <c r="A139" s="38">
         <v>40</v>
       </c>
@@ -8480,7 +8193,7 @@
       </c>
       <c r="G139" s="39"/>
       <c r="H139" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I139" s="96"/>
@@ -8489,12 +8202,12 @@
       <c r="L139" s="100"/>
       <c r="M139" s="100"/>
       <c r="N139" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O139" s="41"/>
     </row>
-    <row r="140" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15" ht="14">
       <c r="A140" s="38">
         <v>50</v>
       </c>
@@ -8513,7 +8226,7 @@
       </c>
       <c r="G140" s="39"/>
       <c r="H140" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I140" s="96"/>
@@ -8522,12 +8235,12 @@
       <c r="L140" s="100"/>
       <c r="M140" s="100"/>
       <c r="N140" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O140" s="41"/>
     </row>
-    <row r="141" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15" ht="14">
       <c r="A141" s="38">
         <v>60</v>
       </c>
@@ -8546,7 +8259,7 @@
       </c>
       <c r="G141" s="39"/>
       <c r="H141" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I141" s="96"/>
@@ -8555,12 +8268,12 @@
       <c r="L141" s="100"/>
       <c r="M141" s="100"/>
       <c r="N141" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O141" s="41"/>
     </row>
-    <row r="142" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15" ht="14">
       <c r="A142" s="38">
         <v>70</v>
       </c>
@@ -8579,7 +8292,7 @@
       </c>
       <c r="G142" s="39"/>
       <c r="H142" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I142" s="96"/>
@@ -8588,12 +8301,12 @@
       <c r="L142" s="100"/>
       <c r="M142" s="100"/>
       <c r="N142" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O142" s="41"/>
     </row>
-    <row r="143" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15" ht="14">
       <c r="A143" s="38">
         <v>80</v>
       </c>
@@ -8614,7 +8327,7 @@
       </c>
       <c r="G143" s="39"/>
       <c r="H143" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I143" s="96"/>
@@ -8623,12 +8336,12 @@
       <c r="L143" s="100"/>
       <c r="M143" s="100"/>
       <c r="N143" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O143" s="41"/>
     </row>
-    <row r="144" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:15" ht="14">
       <c r="A144" s="38">
         <v>90</v>
       </c>
@@ -8649,7 +8362,7 @@
       </c>
       <c r="G144" s="39"/>
       <c r="H144" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I144" s="96"/>
@@ -8658,12 +8371,12 @@
       <c r="L144" s="100"/>
       <c r="M144" s="100"/>
       <c r="N144" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O144" s="41"/>
     </row>
-    <row r="145" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:15" ht="14">
       <c r="A145" s="38">
         <v>100</v>
       </c>
@@ -8682,7 +8395,7 @@
       </c>
       <c r="G145" s="39"/>
       <c r="H145" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I145" s="96"/>
@@ -8691,12 +8404,12 @@
       <c r="L145" s="100"/>
       <c r="M145" s="100"/>
       <c r="N145" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O145" s="41"/>
     </row>
-    <row r="146" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:15" ht="14">
       <c r="A146" s="38">
         <v>110</v>
       </c>
@@ -8717,7 +8430,7 @@
       </c>
       <c r="G146" s="39"/>
       <c r="H146" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I146" s="96"/>
@@ -8726,12 +8439,12 @@
       <c r="L146" s="100"/>
       <c r="M146" s="100"/>
       <c r="N146" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O146" s="41"/>
     </row>
-    <row r="147" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:15" ht="14">
       <c r="A147" s="38">
         <v>120</v>
       </c>
@@ -8752,7 +8465,7 @@
       </c>
       <c r="G147" s="39"/>
       <c r="H147" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I147" s="96"/>
@@ -8761,12 +8474,12 @@
       <c r="L147" s="100"/>
       <c r="M147" s="100"/>
       <c r="N147" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O147" s="41"/>
     </row>
-    <row r="148" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:15" ht="14">
       <c r="A148" s="38">
         <v>130</v>
       </c>
@@ -8785,7 +8498,7 @@
       </c>
       <c r="G148" s="42"/>
       <c r="H148" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.5625</v>
       </c>
       <c r="I148" s="96">
@@ -8798,14 +8511,14 @@
       <c r="L148" s="100"/>
       <c r="M148" s="100"/>
       <c r="N148" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.125</v>
       </c>
       <c r="O148" s="155" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15" ht="14">
       <c r="A149" s="38">
         <v>140</v>
       </c>
@@ -8826,7 +8539,7 @@
       </c>
       <c r="G149" s="42"/>
       <c r="H149" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>12.911833575599999</v>
       </c>
       <c r="I149" s="96">
@@ -8843,14 +8556,14 @@
         <v>0.5</v>
       </c>
       <c r="N149" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>25.823667151199999</v>
       </c>
       <c r="O149" s="155">
         <v>70901</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15" ht="14">
       <c r="A150" s="38">
         <v>150</v>
       </c>
@@ -8871,7 +8584,7 @@
       </c>
       <c r="G150" s="42"/>
       <c r="H150" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>16.25</v>
       </c>
       <c r="I150" s="96">
@@ -8884,14 +8597,14 @@
       <c r="L150" s="100"/>
       <c r="M150" s="100"/>
       <c r="N150" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>97.5</v>
       </c>
       <c r="O150" s="155">
         <v>70902</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:15" ht="14">
       <c r="A151" s="38">
         <v>160</v>
       </c>
@@ -8910,7 +8623,7 @@
       </c>
       <c r="G151" s="42"/>
       <c r="H151" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I151" s="96"/>
@@ -8919,12 +8632,12 @@
       <c r="L151" s="100"/>
       <c r="M151" s="100"/>
       <c r="N151" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O151" s="41"/>
     </row>
-    <row r="152" spans="1:15" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:15" s="2" customFormat="1" ht="14">
       <c r="A152" s="38">
         <v>170</v>
       </c>
@@ -8945,7 +8658,7 @@
       </c>
       <c r="G152" s="42"/>
       <c r="H152" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I152" s="96"/>
@@ -8954,12 +8667,12 @@
       <c r="L152" s="100"/>
       <c r="M152" s="100"/>
       <c r="N152" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O152" s="41"/>
     </row>
-    <row r="153" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15" ht="14">
       <c r="A153" s="38">
         <v>180</v>
       </c>
@@ -8980,7 +8693,7 @@
       </c>
       <c r="G153" s="42"/>
       <c r="H153" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I153" s="96"/>
@@ -8989,12 +8702,12 @@
       <c r="L153" s="100"/>
       <c r="M153" s="100"/>
       <c r="N153" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O153" s="41"/>
     </row>
-    <row r="154" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" ht="14">
       <c r="A154" s="38">
         <v>190</v>
       </c>
@@ -9013,7 +8726,7 @@
       </c>
       <c r="G154" s="39"/>
       <c r="H154" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I154" s="96"/>
@@ -9022,12 +8735,12 @@
       <c r="L154" s="100"/>
       <c r="M154" s="100"/>
       <c r="N154" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O154" s="41"/>
     </row>
-    <row r="155" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" ht="14">
       <c r="A155" s="38">
         <v>200</v>
       </c>
@@ -9048,7 +8761,7 @@
       </c>
       <c r="G155" s="42"/>
       <c r="H155" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I155" s="96"/>
@@ -9057,12 +8770,12 @@
       <c r="L155" s="100"/>
       <c r="M155" s="100"/>
       <c r="N155" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O155" s="41"/>
     </row>
-    <row r="156" spans="1:15" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15" s="4" customFormat="1" ht="14">
       <c r="A156" s="38">
         <v>210</v>
       </c>
@@ -9083,7 +8796,7 @@
       </c>
       <c r="G156" s="42"/>
       <c r="H156" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I156" s="96"/>
@@ -9092,12 +8805,12 @@
       <c r="L156" s="100"/>
       <c r="M156" s="100"/>
       <c r="N156" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O156" s="41"/>
     </row>
-    <row r="157" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" ht="14">
       <c r="A157" s="38">
         <v>220</v>
       </c>
@@ -9116,7 +8829,7 @@
       </c>
       <c r="G157" s="39"/>
       <c r="H157" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I157" s="96"/>
@@ -9125,12 +8838,12 @@
       <c r="L157" s="100"/>
       <c r="M157" s="100"/>
       <c r="N157" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O157" s="41"/>
     </row>
-    <row r="158" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" ht="14">
       <c r="A158" s="38">
         <v>230</v>
       </c>
@@ -9151,7 +8864,7 @@
       </c>
       <c r="G158" s="42"/>
       <c r="H158" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I158" s="96"/>
@@ -9160,12 +8873,12 @@
       <c r="L158" s="100"/>
       <c r="M158" s="100"/>
       <c r="N158" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O158" s="41"/>
     </row>
-    <row r="159" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" ht="14">
       <c r="A159" s="38">
         <v>240</v>
       </c>
@@ -9186,7 +8899,7 @@
       </c>
       <c r="G159" s="42"/>
       <c r="H159" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I159" s="96"/>
@@ -9195,12 +8908,12 @@
       <c r="L159" s="100"/>
       <c r="M159" s="100"/>
       <c r="N159" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O159" s="41"/>
     </row>
-    <row r="160" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" ht="14">
       <c r="A160" s="38">
         <v>250</v>
       </c>
@@ -9219,7 +8932,7 @@
       </c>
       <c r="G160" s="39"/>
       <c r="H160" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I160" s="96"/>
@@ -9228,12 +8941,12 @@
       <c r="L160" s="100"/>
       <c r="M160" s="100"/>
       <c r="N160" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O160" s="41"/>
     </row>
-    <row r="161" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" ht="14">
       <c r="A161" s="38">
         <v>260</v>
       </c>
@@ -9254,7 +8967,7 @@
       </c>
       <c r="G161" s="42"/>
       <c r="H161" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I161" s="96"/>
@@ -9263,12 +8976,12 @@
       <c r="L161" s="100"/>
       <c r="M161" s="100"/>
       <c r="N161" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O161" s="41"/>
     </row>
-    <row r="162" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" ht="14">
       <c r="A162" s="38">
         <v>270</v>
       </c>
@@ -9289,7 +9002,7 @@
       </c>
       <c r="G162" s="42"/>
       <c r="H162" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I162" s="96"/>
@@ -9298,12 +9011,12 @@
       <c r="L162" s="100"/>
       <c r="M162" s="100"/>
       <c r="N162" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O162" s="41"/>
     </row>
-    <row r="163" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" ht="14">
       <c r="A163" s="38">
         <v>280</v>
       </c>
@@ -9322,7 +9035,7 @@
       </c>
       <c r="G163" s="39"/>
       <c r="H163" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I163" s="96"/>
@@ -9331,12 +9044,12 @@
       <c r="L163" s="100"/>
       <c r="M163" s="100"/>
       <c r="N163" s="112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O163" s="41"/>
     </row>
-    <row r="164" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" ht="14">
       <c r="A164" s="38">
         <v>290</v>
       </c>
@@ -9369,7 +9082,7 @@
       </c>
       <c r="O164" s="41"/>
     </row>
-    <row r="165" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" ht="14">
       <c r="A165" s="38">
         <v>300</v>
       </c>
@@ -9402,7 +9115,7 @@
       </c>
       <c r="O165" s="41"/>
     </row>
-    <row r="166" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="15" thickBot="1">
       <c r="A166" s="38">
         <v>310</v>
       </c>
@@ -9435,7 +9148,7 @@
       </c>
       <c r="O166" s="41"/>
     </row>
-    <row r="167" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A167" s="9"/>
       <c r="B167" s="53" t="s">
         <v>77</v>
@@ -9471,7 +9184,7 @@
       </c>
       <c r="O167" s="12"/>
     </row>
-    <row r="168" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" ht="15" thickTop="1">
       <c r="A168" s="43">
         <v>10</v>
       </c>
@@ -9490,7 +9203,7 @@
       </c>
       <c r="G168" s="44"/>
       <c r="H168" s="45">
-        <f t="shared" ref="H168:H181" si="15">SUM(J168:M168)</f>
+        <f t="shared" ref="H168:H181" si="17">SUM(J168:M168)</f>
         <v>0</v>
       </c>
       <c r="I168" s="97"/>
@@ -9499,12 +9212,12 @@
       <c r="L168" s="106"/>
       <c r="M168" s="106"/>
       <c r="N168" s="113">
-        <f t="shared" ref="N168:N181" si="16">H168*I168</f>
+        <f t="shared" ref="N168:N181" si="18">H168*I168</f>
         <v>0</v>
       </c>
       <c r="O168" s="46"/>
     </row>
-    <row r="169" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" ht="14">
       <c r="A169" s="43">
         <v>20</v>
       </c>
@@ -9525,7 +9238,7 @@
       </c>
       <c r="G169" s="44"/>
       <c r="H169" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>85</v>
       </c>
       <c r="I169" s="97">
@@ -9538,12 +9251,12 @@
       <c r="L169" s="106"/>
       <c r="M169" s="106"/>
       <c r="N169" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>340</v>
       </c>
       <c r="O169" s="46"/>
     </row>
-    <row r="170" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" ht="14">
       <c r="A170" s="43">
         <v>30</v>
       </c>
@@ -9564,7 +9277,7 @@
       </c>
       <c r="G170" s="44"/>
       <c r="H170" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I170" s="97"/>
@@ -9573,12 +9286,12 @@
       <c r="L170" s="106"/>
       <c r="M170" s="106"/>
       <c r="N170" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O170" s="46"/>
     </row>
-    <row r="171" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" ht="14">
       <c r="A171" s="43">
         <v>40</v>
       </c>
@@ -9599,7 +9312,7 @@
       </c>
       <c r="G171" s="44"/>
       <c r="H171" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I171" s="97"/>
@@ -9608,12 +9321,12 @@
       <c r="L171" s="106"/>
       <c r="M171" s="106"/>
       <c r="N171" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O171" s="46"/>
     </row>
-    <row r="172" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" ht="14">
       <c r="A172" s="43">
         <v>50</v>
       </c>
@@ -9634,7 +9347,7 @@
       </c>
       <c r="G172" s="47"/>
       <c r="H172" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I172" s="97"/>
@@ -9643,12 +9356,12 @@
       <c r="L172" s="106"/>
       <c r="M172" s="106"/>
       <c r="N172" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O172" s="46"/>
     </row>
-    <row r="173" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" ht="14">
       <c r="A173" s="43">
         <v>60</v>
       </c>
@@ -9667,7 +9380,7 @@
       </c>
       <c r="G173" s="44"/>
       <c r="H173" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I173" s="97"/>
@@ -9676,12 +9389,12 @@
       <c r="L173" s="106"/>
       <c r="M173" s="106"/>
       <c r="N173" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O173" s="46"/>
     </row>
-    <row r="174" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" ht="14">
       <c r="A174" s="43">
         <v>70</v>
       </c>
@@ -9700,7 +9413,7 @@
       </c>
       <c r="G174" s="44"/>
       <c r="H174" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I174" s="97"/>
@@ -9709,12 +9422,12 @@
       <c r="L174" s="106"/>
       <c r="M174" s="106"/>
       <c r="N174" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O174" s="46"/>
     </row>
-    <row r="175" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" ht="14">
       <c r="A175" s="43">
         <v>80</v>
       </c>
@@ -9735,7 +9448,7 @@
       </c>
       <c r="G175" s="44"/>
       <c r="H175" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I175" s="97"/>
@@ -9744,12 +9457,12 @@
       <c r="L175" s="106"/>
       <c r="M175" s="106"/>
       <c r="N175" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O175" s="46"/>
     </row>
-    <row r="176" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15" ht="14">
       <c r="A176" s="43">
         <v>90</v>
       </c>
@@ -9770,7 +9483,7 @@
       </c>
       <c r="G176" s="44"/>
       <c r="H176" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I176" s="97"/>
@@ -9779,12 +9492,12 @@
       <c r="L176" s="106"/>
       <c r="M176" s="106"/>
       <c r="N176" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O176" s="46"/>
     </row>
-    <row r="177" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15" ht="14">
       <c r="A177" s="43">
         <v>100</v>
       </c>
@@ -9803,7 +9516,7 @@
       </c>
       <c r="G177" s="44"/>
       <c r="H177" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I177" s="97"/>
@@ -9812,12 +9525,12 @@
       <c r="L177" s="106"/>
       <c r="M177" s="106"/>
       <c r="N177" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O177" s="46"/>
     </row>
-    <row r="178" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15" ht="14">
       <c r="A178" s="43">
         <v>110</v>
       </c>
@@ -9838,7 +9551,7 @@
       </c>
       <c r="G178" s="44"/>
       <c r="H178" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I178" s="97"/>
@@ -9847,12 +9560,12 @@
       <c r="L178" s="106"/>
       <c r="M178" s="106"/>
       <c r="N178" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O178" s="46"/>
     </row>
-    <row r="179" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" ht="14">
       <c r="A179" s="43">
         <v>120</v>
       </c>
@@ -9873,7 +9586,7 @@
       </c>
       <c r="G179" s="44"/>
       <c r="H179" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I179" s="97"/>
@@ -9882,12 +9595,12 @@
       <c r="L179" s="106"/>
       <c r="M179" s="106"/>
       <c r="N179" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O179" s="46"/>
     </row>
-    <row r="180" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15" ht="14">
       <c r="A180" s="43">
         <v>130</v>
       </c>
@@ -9906,7 +9619,7 @@
       </c>
       <c r="G180" s="44"/>
       <c r="H180" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I180" s="97"/>
@@ -9915,12 +9628,12 @@
       <c r="L180" s="106"/>
       <c r="M180" s="106"/>
       <c r="N180" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O180" s="46"/>
     </row>
-    <row r="181" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="15" thickBot="1">
       <c r="A181" s="43">
         <v>140</v>
       </c>
@@ -9939,7 +9652,7 @@
       </c>
       <c r="G181" s="44"/>
       <c r="H181" s="45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I181" s="97"/>
@@ -9948,12 +9661,12 @@
       <c r="L181" s="106"/>
       <c r="M181" s="106"/>
       <c r="N181" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O181" s="46"/>
     </row>
-    <row r="182" spans="1:15" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A182" s="9"/>
       <c r="B182" s="53" t="s">
         <v>76</v>
@@ -9989,7 +9702,7 @@
       </c>
       <c r="O182" s="12"/>
     </row>
-    <row r="183" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" ht="16" thickTop="1" thickBot="1">
       <c r="A183" s="120"/>
       <c r="B183" s="122" t="s">
         <v>34</v>
@@ -10005,27 +9718,27 @@
       <c r="I183" s="121"/>
       <c r="J183" s="125">
         <f>J182+J167+J135+J121+J36+J81+J97+J111</f>
-        <v>1917.9685332971069</v>
+        <v>605.00726715120004</v>
       </c>
       <c r="K183" s="125">
         <f>K182+K167+K135+K121+K36+K81+K97+K111</f>
-        <v>523.37342423828795</v>
+        <v>331.66139999999996</v>
       </c>
       <c r="L183" s="125">
         <f>L182+L167+L135+L121+L36+L81+L97+L111</f>
-        <v>2.406438067726647</v>
+        <v>0</v>
       </c>
       <c r="M183" s="125">
         <f>M182+M167+M135+M121+M36+M81+M97+M111</f>
-        <v>30.776666666666667</v>
+        <v>30.11</v>
       </c>
       <c r="N183" s="125">
         <f>N182+N167+N135+N121+N36+N81+N97+N111</f>
-        <v>2474.5250622697886</v>
+        <v>966.77866715120001</v>
       </c>
       <c r="O183" s="121"/>
     </row>
-    <row r="184" spans="1:15" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15" ht="14" thickTop="1">
       <c r="A184" s="3"/>
       <c r="B184" s="61"/>
       <c r="C184" s="1"/>
@@ -10041,7 +9754,7 @@
       <c r="M184" s="1"/>
       <c r="N184" s="1"/>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15">
       <c r="A185" s="3"/>
       <c r="B185" s="61"/>
       <c r="C185" s="1"/>
@@ -10057,7 +9770,7 @@
       <c r="M185" s="1"/>
       <c r="N185" s="1"/>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15">
       <c r="A186" s="7"/>
       <c r="B186" s="3"/>
       <c r="O186" s="4"/>

</xml_diff>